<commit_message>
Parse ignored sectors file
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/names_to_be_ignored.xlsx
+++ b/logic/test/data/_input/05_model_parameters/names_to_be_ignored.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Unit_RMA\MAP\_Modellen\E-MAP\05_Runs\_input\05_model_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCB54C-6829-4376-A5E2-94CA9AA4595B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6BB45C-E37E-42A7-B533-A7361DFC491B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="2100" yWindow="1170" windowWidth="20910" windowHeight="13125" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,16 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>pollutant_names</t>
-  </si>
-  <si>
-    <t>NFR_names</t>
-  </si>
-  <si>
-    <t>GNFR_names</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>1A3ai(ii)</t>
   </si>
@@ -80,6 +71,9 @@
   </si>
   <si>
     <t>N_Natural</t>
+  </si>
+  <si>
+    <t>names</t>
   </si>
 </sst>
 </file>
@@ -145,7 +139,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant_ignore" displayName="tbl_pollutant_ignore" ref="A1:A2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:A2" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
   <tableColumns count="1">
-    <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="pollutant_names"/>
+    <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="names"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -155,7 +149,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FDCE720D-A617-4F5B-8433-85E2C6857173}" name="tbl_NFR_ignore" displayName="tbl_NFR_ignore" ref="A1:A9" totalsRowShown="0">
   <autoFilter ref="A1:A9" xr:uid="{BD0EA715-BDB1-4D0E-80B6-1F3E5150B3C3}"/>
   <tableColumns count="1">
-    <tableColumn id="2" xr3:uid="{ECCCA51A-7F4A-4651-8972-626FD9996640}" name="NFR_names"/>
+    <tableColumn id="2" xr3:uid="{ECCCA51A-7F4A-4651-8972-626FD9996640}" name="names"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -165,7 +159,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DDFAB383-A4A3-4E60-ACBF-A17081708E8F}" name="tbl_GNFR" displayName="tbl_GNFR" ref="A1:A5" totalsRowShown="0">
   <autoFilter ref="A1:A5" xr:uid="{77712CCD-413A-4A46-839B-37AAA553DFC3}"/>
   <tableColumns count="1">
-    <tableColumn id="2" xr3:uid="{55D6EFA0-D345-4DC4-92DA-74FD0EA0E1C2}" name="GNFR_names"/>
+    <tableColumn id="2" xr3:uid="{55D6EFA0-D345-4DC4-92DA-74FD0EA0E1C2}" name="names"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -470,9 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -481,7 +473,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -497,9 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F794111A-ABDF-4210-BBBE-1B707CBC36D1}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -508,47 +498,47 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -563,9 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA1389C-35B1-417E-B6AE-DDCDA0344782}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -574,27 +562,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Respect ignored pollutants, calculate PMcoarse for non flanders inputs
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/05_model_parameters/names_to_be_ignored.xlsx
+++ b/logic/test/data/_input/05_model_parameters/names_to_be_ignored.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\E-MAP\05_Runs\_input\05_model_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\projects\E-MAP\05_Runs\_input\05_model_parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6BB45C-E37E-42A7-B533-A7361DFC491B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A3658-3C43-4897-93C6-8474E7D5F04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1170" windowWidth="20910" windowHeight="13125" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12251410-17C7-4612-87CA-5DF1EC65E2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="pollutant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>1A3ai(ii)</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>names</t>
+  </si>
+  <si>
+    <t>PMcoarse</t>
   </si>
 </sst>
 </file>
@@ -136,7 +139,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant_ignore" displayName="tbl_pollutant_ignore" ref="A1:A2" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4A88631E-3733-463E-AE4E-37BF456FD3D8}" name="tbl_pollutant_ignore" displayName="tbl_pollutant_ignore" ref="A1:A2" totalsRowShown="0">
   <autoFilter ref="A1:A2" xr:uid="{A508361B-4E71-4F87-8B57-2CE0238DA6A9}"/>
   <tableColumns count="1">
     <tableColumn id="2" xr3:uid="{06197840-3C9F-4555-BD99-57AE89CFAE84}" name="names"/>
@@ -462,9 +465,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BD3C6-51C2-4B17-80FA-10EB7A062B80}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -474,6 +479,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>